<commit_message>
add lab and 30
</commit_message>
<xml_diff>
--- a/Lab/02/excel/data.xlsx
+++ b/Lab/02/excel/data.xlsx
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.8104182846759259</v>
+        <v>0.9876501441435186</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -486,7 +486,7 @@
         </is>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.8104182846759259</v>
+        <v>0.9876501441435186</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>

</xml_diff>